<commit_message>
Added checkFirstMoveCenter Changed the parameter of makeMove to String array
</commit_message>
<xml_diff>
--- a/ScrabbleBoardLayout.xlsx
+++ b/ScrabbleBoardLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\MASTER\UniversityofTwente\PreMaster\PreMasterQ2\Programming\Project\Scrabble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BCAC12-1361-4383-AC55-2E0B37AE0CC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9439A945-63C9-4990-89ED-47D88A6FA304}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" xr2:uid="{734D654A-568C-497E-B9DD-81E14E59DC01}"/>
   </bookViews>
@@ -25,18 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="4">
-  <si>
-    <t>3W</t>
-  </si>
-  <si>
-    <t>2W</t>
-  </si>
-  <si>
-    <t>3L</t>
-  </si>
-  <si>
-    <t>2L</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -465,7 +495,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="15" width="4.6640625" style="1" customWidth="1"/>
+    <col min="1" max="15" width="3.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -561,7 +591,9 @@
       <c r="E6" s="3"/>
       <c r="F6" s="6"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="6"/>
       <c r="K6" s="3"/>
@@ -578,7 +610,9 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -593,10 +627,18 @@
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="4"/>
@@ -612,9 +654,15 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="4"/>
@@ -627,11 +675,21 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -643,9 +701,15 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -660,7 +724,9 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="4"/>
@@ -677,7 +743,9 @@
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="3"/>
@@ -694,7 +762,9 @@
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -707,11 +777,21 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>

</xml_diff>

<commit_message>
Example board for testing purposes
</commit_message>
<xml_diff>
--- a/ScrabbleBoardLayout.xlsx
+++ b/ScrabbleBoardLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\MASTER\UniversityofTwente\PreMaster\PreMasterQ2\Programming\Project\Scrabble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9439A945-63C9-4990-89ED-47D88A6FA304}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E29790A-55C8-4531-A117-A077973D2166}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" xr2:uid="{734D654A-568C-497E-B9DD-81E14E59DC01}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>D</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -741,16 +747,30 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="5"/>

</xml_diff>